<commit_message>
updated per Meeshes comments
</commit_message>
<xml_diff>
--- a/SuppTables/Supp. Table 9 - HPO_GO_Enrichment.xlsx
+++ b/SuppTables/Supp. Table 9 - HPO_GO_Enrichment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gdrive\umn\UMN\Documents\Manuscripts\ZmIonome Manuscript\WorkingDraft\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\CamocoManuscript\SuppTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -334,7 +334,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,7 +345,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -356,7 +370,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -364,29 +378,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,24 +700,25 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.28515625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -743,1574 +751,1575 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="4">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
         <v>27</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>71</v>
       </c>
-      <c r="F2">
-        <v>16953</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G2" s="4">
         <v>5.6728053973108877E-3</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="H2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
         <v>27</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>71</v>
       </c>
-      <c r="F3">
-        <v>16953</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G3" s="4">
         <v>5.6728053973108877E-3</v>
       </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="H3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
         <v>27</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>85</v>
       </c>
-      <c r="F4">
-        <v>16953</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G4" s="4">
         <v>8.0388701275701836E-3</v>
       </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="H4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4">
         <v>27</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>99</v>
       </c>
-      <c r="F5">
-        <v>16953</v>
-      </c>
-      <c r="G5">
+      <c r="F5" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G5" s="4">
         <v>1.077507480471728E-2</v>
       </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="H5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
         <v>27</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>101</v>
       </c>
-      <c r="F6">
-        <v>16953</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G6" s="4">
         <v>1.119522203754322E-2</v>
       </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="H6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
         <v>27</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>120</v>
       </c>
-      <c r="F7">
-        <v>16953</v>
-      </c>
-      <c r="G7">
+      <c r="F7" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G7" s="4">
         <v>1.55379477799725E-2</v>
       </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="H7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
         <v>27</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>145</v>
       </c>
-      <c r="F8">
-        <v>16953</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G8" s="4">
         <v>2.2173235469362819E-2</v>
       </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="H8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>126</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>73</v>
       </c>
-      <c r="F9">
-        <v>16953</v>
-      </c>
-      <c r="G9">
+      <c r="F9" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G9" s="4">
         <v>1.7091779210441919E-2</v>
       </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="H9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>3</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>126</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>73</v>
       </c>
-      <c r="F10">
-        <v>16953</v>
-      </c>
-      <c r="G10">
+      <c r="F10" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G10" s="4">
         <v>1.7091779210441919E-2</v>
       </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="H10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>126</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>73</v>
       </c>
-      <c r="F11">
-        <v>16953</v>
-      </c>
-      <c r="G11">
+      <c r="F11" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G11" s="4">
         <v>1.7091779210441919E-2</v>
       </c>
-      <c r="H11" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="H11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>3</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>126</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>77</v>
       </c>
-      <c r="F12">
-        <v>16953</v>
-      </c>
-      <c r="G12">
+      <c r="F12" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G12" s="4">
         <v>1.967829043165515E-2</v>
       </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="H12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>3</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>126</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>81</v>
       </c>
-      <c r="F13">
-        <v>16953</v>
-      </c>
-      <c r="G13">
+      <c r="F13" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G13" s="4">
         <v>2.246909856215594E-2</v>
       </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="H13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>3</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>126</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <v>83</v>
       </c>
-      <c r="F14">
-        <v>16953</v>
-      </c>
-      <c r="G14">
+      <c r="F14" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G14" s="4">
         <v>2.3941232602513171E-2</v>
       </c>
-      <c r="H14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="H14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>3</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>126</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <v>98</v>
       </c>
-      <c r="F15">
-        <v>16953</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G15" s="4">
         <v>3.6605231913178451E-2</v>
       </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="H15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>3</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>126</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4">
         <v>100</v>
       </c>
-      <c r="F16">
-        <v>16953</v>
-      </c>
-      <c r="G16">
+      <c r="F16" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G16" s="4">
         <v>3.8507981690921782E-2</v>
       </c>
-      <c r="H16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="H16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>3</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>126</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <v>100</v>
       </c>
-      <c r="F17">
-        <v>16953</v>
-      </c>
-      <c r="G17">
+      <c r="F17" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G17" s="4">
         <v>3.8507981690921782E-2</v>
       </c>
-      <c r="H17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="H17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>3</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>126</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="4">
         <v>102</v>
       </c>
-      <c r="F18">
-        <v>16953</v>
-      </c>
-      <c r="G18">
+      <c r="F18" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G18" s="4">
         <v>4.046037491780468E-2</v>
       </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="H18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>3</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>126</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="4">
         <v>102</v>
       </c>
-      <c r="F19">
-        <v>16953</v>
-      </c>
-      <c r="G19">
+      <c r="F19" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G19" s="4">
         <v>4.046037491780468E-2</v>
       </c>
-      <c r="H19" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="H19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>3</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>126</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="4">
         <v>108</v>
       </c>
-      <c r="F20">
-        <v>16953</v>
-      </c>
-      <c r="G20">
+      <c r="F20" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G20" s="4">
         <v>4.6612188526688449E-2</v>
       </c>
-      <c r="H20" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="H20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>3</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>126</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="4">
         <v>108</v>
       </c>
-      <c r="F21">
-        <v>16953</v>
-      </c>
-      <c r="G21">
+      <c r="F21" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G21" s="4">
         <v>4.6612188526688449E-2</v>
       </c>
-      <c r="H21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="H21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <v>3</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="4">
         <v>26</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="4">
         <v>153</v>
       </c>
-      <c r="F22">
-        <v>16953</v>
-      </c>
-      <c r="G22">
+      <c r="F22" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G22" s="4">
         <v>1.609165342560546E-3</v>
       </c>
-      <c r="H22" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="H22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>3</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <v>26</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="4">
         <v>153</v>
       </c>
-      <c r="F23">
-        <v>16953</v>
-      </c>
-      <c r="G23">
+      <c r="F23" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G23" s="4">
         <v>1.609165342560546E-3</v>
       </c>
-      <c r="H23" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="H23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="4">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4">
         <v>26</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="4">
         <v>150</v>
       </c>
-      <c r="F24">
-        <v>16953</v>
-      </c>
-      <c r="G24">
+      <c r="F24" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G24" s="4">
         <v>2.199552441429338E-2</v>
       </c>
-      <c r="H24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="H24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="4">
+        <v>2</v>
+      </c>
+      <c r="D25" s="4">
         <v>26</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="4">
         <v>162</v>
       </c>
-      <c r="F25">
-        <v>16953</v>
-      </c>
-      <c r="G25">
+      <c r="F25" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G25" s="4">
         <v>2.5382508491766761E-2</v>
       </c>
-      <c r="H25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="H25" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
+      <c r="C26" s="4">
+        <v>2</v>
+      </c>
+      <c r="D26" s="4">
         <v>26</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="4">
         <v>209</v>
       </c>
-      <c r="F26">
-        <v>16953</v>
-      </c>
-      <c r="G26">
+      <c r="F26" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G26" s="4">
         <v>4.0495073959185987E-2</v>
       </c>
-      <c r="H26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="H26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="4">
         <v>4</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <v>76</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="4">
         <v>79</v>
       </c>
-      <c r="F27">
-        <v>16953</v>
-      </c>
-      <c r="G27">
+      <c r="F27" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G27" s="4">
         <v>4.3443503542755932E-4</v>
       </c>
-      <c r="H27" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="H27" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="4">
         <v>4</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="4">
         <v>76</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="4">
         <v>79</v>
       </c>
-      <c r="F28">
-        <v>16953</v>
-      </c>
-      <c r="G28">
+      <c r="F28" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G28" s="4">
         <v>4.3443503542755932E-4</v>
       </c>
-      <c r="H28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="H28" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
+      <c r="C29" s="4">
+        <v>2</v>
+      </c>
+      <c r="D29" s="4">
         <v>76</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="4">
         <v>31</v>
       </c>
-      <c r="F29">
-        <v>16953</v>
-      </c>
-      <c r="G29">
+      <c r="F29" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G29" s="4">
         <v>8.4784937050692965E-3</v>
       </c>
-      <c r="H29" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="H29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30">
+      <c r="C30" s="4">
+        <v>2</v>
+      </c>
+      <c r="D30" s="4">
         <v>76</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="4">
         <v>31</v>
       </c>
-      <c r="F30">
-        <v>16953</v>
-      </c>
-      <c r="G30">
+      <c r="F30" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G30" s="4">
         <v>8.4784937050692965E-3</v>
       </c>
-      <c r="H30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="H30" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
+      <c r="C31" s="4">
+        <v>2</v>
+      </c>
+      <c r="D31" s="4">
         <v>76</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="4">
         <v>31</v>
       </c>
-      <c r="F31">
-        <v>16953</v>
-      </c>
-      <c r="G31">
+      <c r="F31" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G31" s="4">
         <v>8.4784937050692965E-3</v>
       </c>
-      <c r="H31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" t="s">
+      <c r="H31" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32">
+      <c r="C32" s="4">
+        <v>2</v>
+      </c>
+      <c r="D32" s="4">
         <v>76</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="4">
         <v>61</v>
       </c>
-      <c r="F32">
-        <v>16953</v>
-      </c>
-      <c r="G32">
+      <c r="F32" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G32" s="4">
         <v>3.0611450596851719E-2</v>
       </c>
-      <c r="H32" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="H32" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33">
+      <c r="C33" s="4">
+        <v>2</v>
+      </c>
+      <c r="D33" s="4">
         <v>76</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="4">
         <v>69</v>
       </c>
-      <c r="F33">
-        <v>16953</v>
-      </c>
-      <c r="G33">
+      <c r="F33" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G33" s="4">
         <v>3.8356877112621812E-2</v>
       </c>
-      <c r="H33" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="H33" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34">
+      <c r="C34" s="4">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4">
         <v>76</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="4">
         <v>73</v>
       </c>
-      <c r="F34">
-        <v>16953</v>
-      </c>
-      <c r="G34">
+      <c r="F34" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G34" s="4">
         <v>4.2480743208483648E-2</v>
       </c>
-      <c r="H34" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="H34" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J34" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35">
+      <c r="C35" s="4">
+        <v>2</v>
+      </c>
+      <c r="D35" s="4">
         <v>76</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="4">
         <v>77</v>
       </c>
-      <c r="F35">
-        <v>16953</v>
-      </c>
-      <c r="G35">
+      <c r="F35" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G35" s="4">
         <v>4.6762689241433571E-2</v>
       </c>
-      <c r="H35" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="H35" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="4">
         <v>4</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="4">
         <v>58</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="4">
         <v>237</v>
       </c>
-      <c r="F36">
-        <v>16953</v>
-      </c>
-      <c r="G36">
+      <c r="F36" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G36" s="4">
         <v>8.7582899104470743E-3</v>
       </c>
-      <c r="H36" t="b">
-        <v>0</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="H36" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J36" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="4">
         <v>4</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="4">
         <v>58</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="4">
         <v>279</v>
       </c>
-      <c r="F37">
-        <v>16953</v>
-      </c>
-      <c r="G37">
+      <c r="F37" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G37" s="4">
         <v>1.5197282616416931E-2</v>
       </c>
-      <c r="H37" t="b">
-        <v>0</v>
-      </c>
-      <c r="I37" t="s">
+      <c r="H37" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38">
+      <c r="C38" s="4">
+        <v>2</v>
+      </c>
+      <c r="D38" s="4">
         <v>58</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="4">
         <v>55</v>
       </c>
-      <c r="F38">
-        <v>16953</v>
-      </c>
-      <c r="G38">
+      <c r="F38" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G38" s="4">
         <v>1.520972332695607E-2</v>
       </c>
-      <c r="H38" t="b">
-        <v>0</v>
-      </c>
-      <c r="I38" t="s">
+      <c r="H38" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39">
+      <c r="C39" s="4">
+        <v>2</v>
+      </c>
+      <c r="D39" s="4">
         <v>58</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="4">
         <v>73</v>
       </c>
-      <c r="F39">
-        <v>16953</v>
-      </c>
-      <c r="G39">
+      <c r="F39" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G39" s="4">
         <v>2.5884258965599649E-2</v>
       </c>
-      <c r="H39" t="b">
-        <v>0</v>
-      </c>
-      <c r="I39" t="s">
+      <c r="H39" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40">
+      <c r="C40" s="4">
+        <v>2</v>
+      </c>
+      <c r="D40" s="4">
         <v>58</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="4">
         <v>73</v>
       </c>
-      <c r="F40">
-        <v>16953</v>
-      </c>
-      <c r="G40">
+      <c r="F40" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G40" s="4">
         <v>2.5884258965599649E-2</v>
       </c>
-      <c r="H40" t="b">
-        <v>0</v>
-      </c>
-      <c r="I40" t="s">
+      <c r="H40" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-      <c r="D41">
+      <c r="C41" s="4">
+        <v>2</v>
+      </c>
+      <c r="D41" s="4">
         <v>58</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="4">
         <v>73</v>
       </c>
-      <c r="F41">
-        <v>16953</v>
-      </c>
-      <c r="G41">
+      <c r="F41" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G41" s="4">
         <v>2.5884258965599649E-2</v>
       </c>
-      <c r="H41" t="b">
-        <v>0</v>
-      </c>
-      <c r="I41" t="s">
+      <c r="H41" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42">
+      <c r="C42" s="4">
+        <v>2</v>
+      </c>
+      <c r="D42" s="4">
         <v>58</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="4">
         <v>77</v>
       </c>
-      <c r="F42">
-        <v>16953</v>
-      </c>
-      <c r="G42">
+      <c r="F42" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G42" s="4">
         <v>2.8570682771111529E-2</v>
       </c>
-      <c r="H42" t="b">
-        <v>0</v>
-      </c>
-      <c r="I42" t="s">
+      <c r="H42" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43">
+      <c r="C43" s="4">
+        <v>2</v>
+      </c>
+      <c r="D43" s="4">
         <v>58</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="4">
         <v>81</v>
       </c>
-      <c r="F43">
-        <v>16953</v>
-      </c>
-      <c r="G43">
+      <c r="F43" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G43" s="4">
         <v>3.1363966425433792E-2</v>
       </c>
-      <c r="H43" t="b">
-        <v>0</v>
-      </c>
-      <c r="I43" t="s">
+      <c r="H43" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44">
+      <c r="C44" s="4">
+        <v>2</v>
+      </c>
+      <c r="D44" s="4">
         <v>58</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="4">
         <v>83</v>
       </c>
-      <c r="F44">
-        <v>16953</v>
-      </c>
-      <c r="G44">
+      <c r="F44" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G44" s="4">
         <v>3.2799646670696757E-2</v>
       </c>
-      <c r="H44" t="b">
-        <v>0</v>
-      </c>
-      <c r="I44" t="s">
+      <c r="H44" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="4">
         <v>3</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="4">
         <v>58</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="4">
         <v>209</v>
       </c>
-      <c r="F45">
-        <v>16953</v>
-      </c>
-      <c r="G45">
+      <c r="F45" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G45" s="4">
         <v>3.4724782031211592E-2</v>
       </c>
-      <c r="H45" t="b">
-        <v>0</v>
-      </c>
-      <c r="I45" t="s">
+      <c r="H45" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J45" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46">
+      <c r="C46" s="4">
+        <v>2</v>
+      </c>
+      <c r="D46" s="4">
         <v>58</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="4">
         <v>98</v>
       </c>
-      <c r="F46">
-        <v>16953</v>
-      </c>
-      <c r="G46">
+      <c r="F46" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G46" s="4">
         <v>4.4352129898147692E-2</v>
       </c>
-      <c r="H46" t="b">
-        <v>0</v>
-      </c>
-      <c r="I46" t="s">
+      <c r="H46" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C47">
-        <v>2</v>
-      </c>
-      <c r="D47">
+      <c r="C47" s="4">
+        <v>2</v>
+      </c>
+      <c r="D47" s="4">
         <v>58</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="4">
         <v>100</v>
       </c>
-      <c r="F47">
-        <v>16953</v>
-      </c>
-      <c r="G47">
+      <c r="F47" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G47" s="4">
         <v>4.5991879361038081E-2</v>
       </c>
-      <c r="H47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I47" t="s">
+      <c r="H47" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48">
+      <c r="C48" s="4">
+        <v>2</v>
+      </c>
+      <c r="D48" s="4">
         <v>58</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="4">
         <v>100</v>
       </c>
-      <c r="F48">
-        <v>16953</v>
-      </c>
-      <c r="G48">
+      <c r="F48" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G48" s="4">
         <v>4.5991879361038081E-2</v>
       </c>
-      <c r="H48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I48" t="s">
+      <c r="H48" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49">
+      <c r="C49" s="4">
+        <v>2</v>
+      </c>
+      <c r="D49" s="4">
         <v>58</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="4">
         <v>102</v>
       </c>
-      <c r="F49">
-        <v>16953</v>
-      </c>
-      <c r="G49">
+      <c r="F49" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G49" s="4">
         <v>4.7653823433669869E-2</v>
       </c>
-      <c r="H49" t="b">
-        <v>0</v>
-      </c>
-      <c r="I49" t="s">
+      <c r="H49" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50">
+      <c r="C50" s="4">
+        <v>2</v>
+      </c>
+      <c r="D50" s="4">
         <v>58</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="4">
         <v>102</v>
       </c>
-      <c r="F50">
-        <v>16953</v>
-      </c>
-      <c r="G50">
+      <c r="F50" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G50" s="4">
         <v>4.7653823433669869E-2</v>
       </c>
-      <c r="H50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I50" t="s">
+      <c r="H50" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="4" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>